<commit_message>
Trabalho final com parte de SO
</commit_message>
<xml_diff>
--- a/relatorio2.xlsx
+++ b/relatorio2.xlsx
@@ -1,18 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{9D550302-4D3A-4C6A-B1F2-FC544061172A}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr documentId="10_ncr:8100000_{7C876AE3-31A3-480B-B636-978108C1AD5E}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView windowHeight="12645" windowWidth="22260" xWindow="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Plan1" sheetId="1" r:id="rId1"/>
+    <sheet name="Plan1" r:id="rId1" sheetId="1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="17">
   <si>
     <t>Método</t>
   </si>
@@ -39,11 +39,45 @@
   <si>
     <t>Tempo (ms)</t>
   </si>
+  <si>
+    <t>Arquivo 10</t>
+  </si>
+  <si>
+    <t>Arquivo 11</t>
+  </si>
+  <si>
+    <t>Arquivo 12</t>
+  </si>
+  <si>
+    <t>Arquivo 13</t>
+  </si>
+  <si>
+    <t>Arquivo 14</t>
+  </si>
+  <si>
+    <t>Arquivo 15</t>
+  </si>
+  <si>
+    <t>Arquivo 16</t>
+  </si>
+  <si>
+    <t>Arquivo 17</t>
+  </si>
+  <si>
+    <t>Arquivo 18</t>
+  </si>
+  <si>
+    <t>Arquivo 19</t>
+  </si>
+  <si>
+    <t>Arquivo 20</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -85,22 +119,28 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+  <cellXfs count="5">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -113,7 +153,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="pt-BR"/>
   <c:roundedCorners val="0"/>
@@ -127,6 +167,31 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr anchor="ctr" anchorCtr="1" rot="0" spcFirstLastPara="1" vert="horz" vertOverflow="ellipsis" wrap="square"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" baseline="0" i="0" kern="1200" spc="0" strike="noStrike" sz="1400" u="none">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pt-BR"/>
+              <a:t>Comparativo</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -136,11 +201,11 @@
         <a:effectLst/>
       </c:spPr>
       <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:bodyPr anchor="ctr" anchorCtr="1" rot="0" spcFirstLastPara="1" vert="horz" vertOverflow="ellipsis" wrap="square"/>
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr b="0" baseline="0" i="0" kern="1200" spc="0" strike="noStrike" sz="1400" u="none">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -168,11 +233,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Plan1!$B$1</c:f>
+              <c:f>Plan1!$A$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Tempo (ms)</c:v>
+                  <c:v>Fila de Prioridade</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -189,48 +254,421 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Plan1!$A$2:$A$5</c:f>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Plan1!$B$1:$L$2</c15:sqref>
+                  </c15:fullRef>
+                  <c15:levelRef>
+                    <c15:sqref>Plan1!$B$1:$L$1</c15:sqref>
+                  </c15:levelRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Plan1!$B$1:$L$1</c:f>
               <c:strCache>
-                <c:ptCount val="4"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>Fila de Prioridade</c:v>
+                  <c:v>Arquivo 10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Menor Primeiro</c:v>
+                  <c:v>Arquivo 11</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Ordem Chegada</c:v>
+                  <c:v>Arquivo 12</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Round Robin</c:v>
+                  <c:v>Arquivo 13</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Arquivo 14</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Arquivo 15</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Arquivo 16</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Arquivo 17</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Arquivo 18</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Arquivo 19</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Arquivo 20</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Plan1!$B$2:$B$5</c:f>
+              <c:f>Plan1!$B$3:$L$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>164</c:v>
+                  <c:v>73</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>78</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>97</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>89</c:v>
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>17</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-84A3-4C3C-A197-E986C185D9A3}"/>
+              <c16:uniqueId val="{00000000-B47C-4CDB-8134-8499B5BD15F5}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Plan1!$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Menor Primeiro</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Plan1!$B$1:$L$2</c15:sqref>
+                  </c15:fullRef>
+                  <c15:levelRef>
+                    <c15:sqref>Plan1!$B$1:$L$1</c15:sqref>
+                  </c15:levelRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Plan1!$B$1:$L$1</c:f>
+              <c:strCache>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>Arquivo 10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Arquivo 11</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Arquivo 12</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Arquivo 13</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Arquivo 14</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Arquivo 15</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Arquivo 16</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Arquivo 17</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Arquivo 18</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Arquivo 19</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Arquivo 20</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Plan1!$B$4:$L$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>19</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-B47C-4CDB-8134-8499B5BD15F5}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Plan1!$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Ordem Chegada</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Plan1!$B$1:$L$2</c15:sqref>
+                  </c15:fullRef>
+                  <c15:levelRef>
+                    <c15:sqref>Plan1!$B$1:$L$1</c15:sqref>
+                  </c15:levelRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Plan1!$B$1:$L$1</c:f>
+              <c:strCache>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>Arquivo 10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Arquivo 11</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Arquivo 12</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Arquivo 13</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Arquivo 14</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Arquivo 15</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Arquivo 16</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Arquivo 17</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Arquivo 18</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Arquivo 19</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Arquivo 20</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Plan1!$B$5:$L$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-B47C-4CDB-8134-8499B5BD15F5}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Plan1!$A$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Round Robin</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Plan1!$B$1:$L$2</c15:sqref>
+                  </c15:fullRef>
+                  <c15:levelRef>
+                    <c15:sqref>Plan1!$B$1:$L$1</c15:sqref>
+                  </c15:levelRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Plan1!$B$1:$L$1</c:f>
+              <c:strCache>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>Arquivo 10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Arquivo 11</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Arquivo 12</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Arquivo 13</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Arquivo 14</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Arquivo 15</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Arquivo 16</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Arquivo 17</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Arquivo 18</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Arquivo 19</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Arquivo 20</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Plan1!$B$6:$L$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>136</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>812</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2533</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-B47C-4CDB-8134-8499B5BD15F5}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -244,11 +682,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="280992840"/>
-        <c:axId val="280990216"/>
+        <c:axId val="463899656"/>
+        <c:axId val="463897360"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="280992840"/>
+        <c:axId val="463899656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -260,7 +698,7 @@
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
             <a:solidFill>
               <a:schemeClr val="tx1">
                 <a:lumMod val="15000"/>
@@ -272,11 +710,11 @@
           <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:bodyPr anchor="ctr" anchorCtr="1" rot="-60000000" spcFirstLastPara="1" vert="horz" vertOverflow="ellipsis" wrap="square"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr b="0" baseline="0" i="0" kern="1200" strike="noStrike" sz="900" u="none">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -291,7 +729,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="280990216"/>
+        <c:crossAx val="463897360"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -299,7 +737,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="280990216"/>
+        <c:axId val="463897360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -307,7 +745,7 @@
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="15000"/>
@@ -331,11 +769,11 @@
           <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:bodyPr anchor="ctr" anchorCtr="1" rot="-60000000" spcFirstLastPara="1" vert="horz" vertOverflow="ellipsis" wrap="square"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr b="0" baseline="0" i="0" kern="1200" strike="noStrike" sz="900" u="none">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -350,7 +788,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="280992840"/>
+        <c:crossAx val="463899656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -362,22 +800,46 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr anchor="ctr" anchorCtr="1" rot="0" spcFirstLastPara="1" vert="horz" vertOverflow="ellipsis" wrap="square"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr b="0" baseline="0" i="0" kern="1200" strike="noStrike" sz="900" u="none">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-BR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
       <a:schemeClr val="bg1"/>
     </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+    <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
       <a:solidFill>
         <a:schemeClr val="tx1">
           <a:lumMod val="15000"/>
@@ -400,7 +862,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+    <c:pageMargins b="0.78740157499999996" footer="0.31496062000000002" header="0.31496062000000002" l="0.511811024" r="0.511811024" t="0.78740157499999996"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -950,26 +1412,26 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+<xdr:wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>14287</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>323850</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>90487</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Gráfico 1">
+        <xdr:cNvPr id="3" name="Gráfico 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4E212F9F-9E30-42F7-8FC8-9E423700FC87}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{259F4374-EDBB-458E-81C0-5D372EE84E6D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -995,10 +1457,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -1033,7 +1495,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic Light"/>
@@ -1068,7 +1530,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic"/>
@@ -1162,21 +1624,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -1193,7 +1655,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -1245,69 +1707,246 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:M6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="A1:B5"/>
+    <sheetView tabSelected="1" workbookViewId="0" zoomScaleNormal="100">
+      <selection activeCell="B1" sqref="B1:L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="16.7109375" collapsed="true"/>
+    <col min="2" max="12" bestFit="true" customWidth="true" width="11.5703125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="4"/>
+      <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="C2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2">
-        <v>164</v>
+      <c r="B3" s="2" t="n">
+        <v>82.0</v>
+      </c>
+      <c r="C3" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="D3" t="n">
+        <v>9.0</v>
+      </c>
+      <c r="E3" t="n">
+        <v>9.0</v>
+      </c>
+      <c r="F3" t="n">
+        <v>9.0</v>
+      </c>
+      <c r="G3" t="n">
+        <v>24.0</v>
+      </c>
+      <c r="H3" t="n">
+        <v>37.0</v>
+      </c>
+      <c r="I3" t="n">
+        <v>54.0</v>
+      </c>
+      <c r="J3" t="n">
+        <v>54.0</v>
+      </c>
+      <c r="K3" t="n">
+        <v>193.0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="2">
-        <v>78</v>
+      <c r="B4" s="2" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="C4" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="D4" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="E4" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="F4" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="G4" t="n">
+        <v>22.0</v>
+      </c>
+      <c r="H4" t="n">
+        <v>31.0</v>
+      </c>
+      <c r="I4" t="n">
+        <v>39.0</v>
+      </c>
+      <c r="J4" t="n">
+        <v>61.0</v>
+      </c>
+      <c r="K4" t="n">
+        <v>171.0</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="2">
-        <v>97</v>
+      <c r="B5" s="2" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D5" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="E5" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="F5" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="G5" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H5" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="I5" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="J5" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="K5" t="n">
+        <v>12.0</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="2">
-        <v>89</v>
+      <c r="B6" s="2" t="n">
+        <v>31.0</v>
+      </c>
+      <c r="C6" t="n">
+        <v>17.0</v>
+      </c>
+      <c r="D6" t="n">
+        <v>31.0</v>
+      </c>
+      <c r="E6" t="n">
+        <v>63.0</v>
+      </c>
+      <c r="F6" t="n">
+        <v>143.0</v>
+      </c>
+      <c r="G6" t="n">
+        <v>578.0</v>
+      </c>
+      <c r="H6" t="n">
+        <v>2106.0</v>
+      </c>
+      <c r="I6" t="n">
+        <v>9028.0</v>
+      </c>
+      <c r="J6" t="n">
+        <v>55591.0</v>
+      </c>
+      <c r="K6" t="n">
+        <v>196396.0</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <mergeCells count="1">
+    <mergeCell ref="A1:A2"/>
+  </mergeCells>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait" paperSize="9" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>